<commit_message>
ajustar exportação de dados para clientes e processos, incluindo tratamento de valores nulos e formatação de datas
</commit_message>
<xml_diff>
--- a/data/output/advbox_processos.xlsx
+++ b/data/output/advbox_processos.xlsx
@@ -581,11 +581,7 @@
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>29/04/2013 18:14</t>
-        </is>
-      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
@@ -642,11 +638,7 @@
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>09/11/2017 16:00</t>
-        </is>
-      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
@@ -703,11 +695,7 @@
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>11/01/2017 13:50</t>
-        </is>
-      </c>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
@@ -760,11 +748,7 @@
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>03/09/2019 15:58</t>
-        </is>
-      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
@@ -797,11 +781,7 @@
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>08/02/2017 18:37</t>
-        </is>
-      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
@@ -854,11 +834,7 @@
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>26/01/2016 17:44</t>
-        </is>
-      </c>
+      <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
@@ -899,11 +875,7 @@
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>10/06/2020 10:51</t>
-        </is>
-      </c>
+      <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
@@ -940,11 +912,7 @@
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>22/06/2016 16:05</t>
-        </is>
-      </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
@@ -993,11 +961,7 @@
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>08/06/2019 22:32</t>
-        </is>
-      </c>
+      <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
@@ -1050,11 +1014,7 @@
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>26/10/2016 16:06</t>
-        </is>
-      </c>
+      <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
@@ -1107,11 +1067,7 @@
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>21/09/2021 09:15</t>
-        </is>
-      </c>
+      <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
@@ -1164,11 +1120,7 @@
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>24/10/2018 11:17</t>
-        </is>
-      </c>
+      <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
@@ -1226,11 +1178,7 @@
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>01/08/2019 10:45</t>
-        </is>
-      </c>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
@@ -1283,11 +1231,7 @@
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>01/12/2016 16:38</t>
-        </is>
-      </c>
+      <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
@@ -1340,11 +1284,7 @@
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>13/12/2016 21:43</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
@@ -1397,11 +1337,7 @@
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>13/11/2014 14:33</t>
-        </is>
-      </c>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
@@ -1454,11 +1390,7 @@
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>19/04/2017 10:53</t>
-        </is>
-      </c>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
@@ -1511,11 +1443,7 @@
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>05/11/2020 10:02</t>
-        </is>
-      </c>
+      <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
@@ -1564,11 +1492,7 @@
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>13/03/2014 17:29</t>
-        </is>
-      </c>
+      <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
@@ -1621,11 +1545,7 @@
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>15/12/2016 17:05</t>
-        </is>
-      </c>
+      <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
@@ -1674,11 +1594,7 @@
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>15/12/2017 13:35</t>
-        </is>
-      </c>
+      <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
@@ -1731,11 +1647,7 @@
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>28/01/2022 14:44</t>
-        </is>
-      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
@@ -1788,11 +1700,7 @@
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>30/08/2012 09:31</t>
-        </is>
-      </c>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
@@ -1833,11 +1741,7 @@
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>26/08/2020 16:46</t>
-        </is>
-      </c>
+      <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
@@ -1890,11 +1794,7 @@
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>29/01/2013 11:52</t>
-        </is>
-      </c>
+      <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
@@ -1947,11 +1847,7 @@
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>14/08/2018 11:10</t>
-        </is>
-      </c>
+      <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
@@ -2000,11 +1896,7 @@
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>23/10/2014 09:51</t>
-        </is>
-      </c>
+      <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
@@ -2053,11 +1945,7 @@
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>16/12/2021 14:09</t>
-        </is>
-      </c>
+      <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
@@ -2094,11 +1982,7 @@
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>01/08/2018 14:44</t>
-        </is>
-      </c>
+      <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
@@ -2151,11 +2035,7 @@
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>29/12/2015 11:26</t>
-        </is>
-      </c>
+      <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
@@ -2212,11 +2092,7 @@
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>21/06/2013 12:14</t>
-        </is>
-      </c>
+      <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
@@ -2269,11 +2145,7 @@
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>12/09/2012 14:29</t>
-        </is>
-      </c>
+      <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
@@ -2314,11 +2186,7 @@
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>22/10/2020 15:44</t>
-        </is>
-      </c>
+      <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
@@ -2371,11 +2239,7 @@
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>24/11/2015 10:26</t>
-        </is>
-      </c>
+      <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
@@ -2428,11 +2292,7 @@
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>03/04/2018 18:17</t>
-        </is>
-      </c>
+      <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
@@ -2485,11 +2345,7 @@
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>05/12/2018 10:09</t>
-        </is>
-      </c>
+      <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
@@ -2546,11 +2402,7 @@
       </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>19/09/2012 14:25</t>
-        </is>
-      </c>
+      <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="inlineStr"/>
@@ -2603,11 +2455,7 @@
       </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>26/07/2017 14:59</t>
-        </is>
-      </c>
+      <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
@@ -2664,11 +2512,7 @@
       </c>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>03/12/2012 11:42</t>
-        </is>
-      </c>
+      <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
@@ -2721,11 +2565,7 @@
       </c>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>28/05/2019 15:03</t>
-        </is>
-      </c>
+      <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
@@ -2778,11 +2618,7 @@
       </c>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>18/04/2019 16:17</t>
-        </is>
-      </c>
+      <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
@@ -2835,11 +2671,7 @@
       </c>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>28/07/2015 11:33</t>
-        </is>
-      </c>
+      <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
@@ -2892,11 +2724,7 @@
       </c>
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>29/09/2016 10:53</t>
-        </is>
-      </c>
+      <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
@@ -2949,11 +2777,7 @@
       </c>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>21/03/2019 14:50</t>
-        </is>
-      </c>
+      <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
@@ -2998,11 +2822,7 @@
       </c>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>25/03/2019 16:29</t>
-        </is>
-      </c>
+      <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
@@ -3055,11 +2875,7 @@
       </c>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>16/07/2015 10:54</t>
-        </is>
-      </c>
+      <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
@@ -3112,11 +2928,7 @@
       </c>
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>13/06/2013 16:13</t>
-        </is>
-      </c>
+      <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
@@ -3169,11 +2981,7 @@
       </c>
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>11/11/2014 14:12</t>
-        </is>
-      </c>
+      <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
@@ -3226,11 +3034,7 @@
       </c>
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>23/10/2019 14:12</t>
-        </is>
-      </c>
+      <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr"/>
@@ -3283,11 +3087,7 @@
       </c>
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>22/05/2017 16:52</t>
-        </is>
-      </c>
+      <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
@@ -3340,11 +3140,7 @@
       </c>
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>08/08/2016 17:37</t>
-        </is>
-      </c>
+      <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr"/>
@@ -3377,11 +3173,7 @@
       </c>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>13/04/2015 11:59</t>
-        </is>
-      </c>
+      <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr"/>
@@ -3434,11 +3226,7 @@
       </c>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>12/09/2014 10:10</t>
-        </is>
-      </c>
+      <c r="O54" t="inlineStr"/>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
       <c r="R54" t="inlineStr"/>
@@ -3491,11 +3279,7 @@
       </c>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr"/>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>11/12/2014 15:37</t>
-        </is>
-      </c>
+      <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="inlineStr"/>
@@ -3548,11 +3332,7 @@
       </c>
       <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr"/>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>30/01/2013 09:59</t>
-        </is>
-      </c>
+      <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
       <c r="R56" t="inlineStr"/>
@@ -3605,11 +3385,7 @@
       </c>
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="inlineStr"/>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>05/12/2012 11:26</t>
-        </is>
-      </c>
+      <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
       <c r="R57" t="inlineStr"/>
@@ -3662,11 +3438,7 @@
       </c>
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr"/>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>17/01/2017 16:18</t>
-        </is>
-      </c>
+      <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="inlineStr"/>
       <c r="R58" t="inlineStr"/>
@@ -3719,11 +3491,7 @@
       </c>
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="inlineStr"/>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>22/04/2021 16:48</t>
-        </is>
-      </c>
+      <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
       <c r="R59" t="inlineStr"/>
@@ -3776,11 +3544,7 @@
       </c>
       <c r="M60" t="inlineStr"/>
       <c r="N60" t="inlineStr"/>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>14/08/2017 20:02</t>
-        </is>
-      </c>
+      <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
       <c r="R60" t="inlineStr"/>
@@ -3833,11 +3597,7 @@
       </c>
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr"/>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>27/01/2014 20:35</t>
-        </is>
-      </c>
+      <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
       <c r="R61" t="inlineStr"/>
@@ -3890,11 +3650,7 @@
       </c>
       <c r="M62" t="inlineStr"/>
       <c r="N62" t="inlineStr"/>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>01/09/2014 15:33</t>
-        </is>
-      </c>
+      <c r="O62" t="inlineStr"/>
       <c r="P62" t="inlineStr"/>
       <c r="Q62" t="inlineStr"/>
       <c r="R62" t="inlineStr"/>
@@ -3943,11 +3699,7 @@
       </c>
       <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr"/>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>09/08/2013 16:35</t>
-        </is>
-      </c>
+      <c r="O63" t="inlineStr"/>
       <c r="P63" t="inlineStr"/>
       <c r="Q63" t="inlineStr"/>
       <c r="R63" t="inlineStr"/>
@@ -4000,11 +3752,7 @@
       </c>
       <c r="M64" t="inlineStr"/>
       <c r="N64" t="inlineStr"/>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>15/05/2014 16:09</t>
-        </is>
-      </c>
+      <c r="O64" t="inlineStr"/>
       <c r="P64" t="inlineStr"/>
       <c r="Q64" t="inlineStr"/>
       <c r="R64" t="inlineStr"/>
@@ -4061,11 +3809,7 @@
       </c>
       <c r="M65" t="inlineStr"/>
       <c r="N65" t="inlineStr"/>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>28/08/2012 11:49</t>
-        </is>
-      </c>
+      <c r="O65" t="inlineStr"/>
       <c r="P65" t="inlineStr"/>
       <c r="Q65" t="inlineStr"/>
       <c r="R65" t="inlineStr"/>
@@ -4118,11 +3862,7 @@
       </c>
       <c r="M66" t="inlineStr"/>
       <c r="N66" t="inlineStr"/>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>07/08/2012 10:09</t>
-        </is>
-      </c>
+      <c r="O66" t="inlineStr"/>
       <c r="P66" t="inlineStr"/>
       <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr"/>
@@ -4179,11 +3919,7 @@
       </c>
       <c r="M67" t="inlineStr"/>
       <c r="N67" t="inlineStr"/>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>30/10/2012 12:56</t>
-        </is>
-      </c>
+      <c r="O67" t="inlineStr"/>
       <c r="P67" t="inlineStr"/>
       <c r="Q67" t="inlineStr"/>
       <c r="R67" t="inlineStr"/>
@@ -4220,11 +3956,7 @@
       </c>
       <c r="M68" t="inlineStr"/>
       <c r="N68" t="inlineStr"/>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>27/08/2019 16:48</t>
-        </is>
-      </c>
+      <c r="O68" t="inlineStr"/>
       <c r="P68" t="inlineStr"/>
       <c r="Q68" t="inlineStr"/>
       <c r="R68" t="inlineStr"/>
@@ -4261,11 +3993,7 @@
       </c>
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr"/>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>02/09/2021 15:45</t>
-        </is>
-      </c>
+      <c r="O69" t="inlineStr"/>
       <c r="P69" t="inlineStr"/>
       <c r="Q69" t="inlineStr"/>
       <c r="R69" t="inlineStr"/>
@@ -4318,11 +4046,7 @@
       </c>
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr"/>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>08/12/2021 17:07</t>
-        </is>
-      </c>
+      <c r="O70" t="inlineStr"/>
       <c r="P70" t="inlineStr"/>
       <c r="Q70" t="inlineStr"/>
       <c r="R70" t="inlineStr"/>
@@ -4375,11 +4099,7 @@
       </c>
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr"/>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>18/02/2021 19:41</t>
-        </is>
-      </c>
+      <c r="O71" t="inlineStr"/>
       <c r="P71" t="inlineStr"/>
       <c r="Q71" t="inlineStr"/>
       <c r="R71" t="inlineStr"/>
@@ -4436,11 +4156,7 @@
       </c>
       <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr"/>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>29/10/2018 15:06</t>
-        </is>
-      </c>
+      <c r="O72" t="inlineStr"/>
       <c r="P72" t="inlineStr"/>
       <c r="Q72" t="inlineStr"/>
       <c r="R72" t="inlineStr"/>
@@ -4493,11 +4209,7 @@
       </c>
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>03/09/2012 16:43</t>
-        </is>
-      </c>
+      <c r="O73" t="inlineStr"/>
       <c r="P73" t="inlineStr"/>
       <c r="Q73" t="inlineStr"/>
       <c r="R73" t="inlineStr"/>
@@ -4550,11 +4262,7 @@
       </c>
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr"/>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>26/01/2016 17:47</t>
-        </is>
-      </c>
+      <c r="O74" t="inlineStr"/>
       <c r="P74" t="inlineStr"/>
       <c r="Q74" t="inlineStr"/>
       <c r="R74" t="inlineStr"/>
@@ -4607,11 +4315,7 @@
       </c>
       <c r="M75" t="inlineStr"/>
       <c r="N75" t="inlineStr"/>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>18/10/2017 12:25</t>
-        </is>
-      </c>
+      <c r="O75" t="inlineStr"/>
       <c r="P75" t="inlineStr"/>
       <c r="Q75" t="inlineStr"/>
       <c r="R75" t="inlineStr"/>
@@ -4664,11 +4368,7 @@
       </c>
       <c r="M76" t="inlineStr"/>
       <c r="N76" t="inlineStr"/>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>26/09/2019 17:21</t>
-        </is>
-      </c>
+      <c r="O76" t="inlineStr"/>
       <c r="P76" t="inlineStr"/>
       <c r="Q76" t="inlineStr"/>
       <c r="R76" t="inlineStr"/>
@@ -4721,11 +4421,7 @@
       </c>
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="inlineStr"/>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>17/09/2014 17:02</t>
-        </is>
-      </c>
+      <c r="O77" t="inlineStr"/>
       <c r="P77" t="inlineStr"/>
       <c r="Q77" t="inlineStr"/>
       <c r="R77" t="inlineStr"/>
@@ -4778,11 +4474,7 @@
       </c>
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="inlineStr"/>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>20/11/2014 11:08</t>
-        </is>
-      </c>
+      <c r="O78" t="inlineStr"/>
       <c r="P78" t="inlineStr"/>
       <c r="Q78" t="inlineStr"/>
       <c r="R78" t="inlineStr"/>
@@ -4840,11 +4532,7 @@
       </c>
       <c r="M79" t="inlineStr"/>
       <c r="N79" t="inlineStr"/>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>30/08/2017 15:37</t>
-        </is>
-      </c>
+      <c r="O79" t="inlineStr"/>
       <c r="P79" t="inlineStr"/>
       <c r="Q79" t="inlineStr"/>
       <c r="R79" t="inlineStr"/>
@@ -4897,11 +4585,7 @@
       </c>
       <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr"/>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>30/10/2015 17:34</t>
-        </is>
-      </c>
+      <c r="O80" t="inlineStr"/>
       <c r="P80" t="inlineStr"/>
       <c r="Q80" t="inlineStr"/>
       <c r="R80" t="inlineStr"/>
@@ -4954,11 +4638,7 @@
       </c>
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr"/>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>16/08/2019 11:17</t>
-        </is>
-      </c>
+      <c r="O81" t="inlineStr"/>
       <c r="P81" t="inlineStr"/>
       <c r="Q81" t="inlineStr"/>
       <c r="R81" t="inlineStr"/>
@@ -5007,11 +4687,7 @@
       </c>
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>28/06/2018 17:58</t>
-        </is>
-      </c>
+      <c r="O82" t="inlineStr"/>
       <c r="P82" t="inlineStr"/>
       <c r="Q82" t="inlineStr"/>
       <c r="R82" t="inlineStr"/>
@@ -5064,11 +4740,7 @@
       </c>
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>19/02/2016 13:53</t>
-        </is>
-      </c>
+      <c r="O83" t="inlineStr"/>
       <c r="P83" t="inlineStr"/>
       <c r="Q83" t="inlineStr"/>
       <c r="R83" t="inlineStr"/>
@@ -5121,11 +4793,7 @@
       </c>
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="inlineStr"/>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>24/07/2014 10:29</t>
-        </is>
-      </c>
+      <c r="O84" t="inlineStr"/>
       <c r="P84" t="inlineStr"/>
       <c r="Q84" t="inlineStr"/>
       <c r="R84" t="inlineStr"/>
@@ -5178,11 +4846,7 @@
       </c>
       <c r="M85" t="inlineStr"/>
       <c r="N85" t="inlineStr"/>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>23/04/2015 15:35</t>
-        </is>
-      </c>
+      <c r="O85" t="inlineStr"/>
       <c r="P85" t="inlineStr"/>
       <c r="Q85" t="inlineStr"/>
       <c r="R85" t="inlineStr"/>
@@ -5235,11 +4899,7 @@
       </c>
       <c r="M86" t="inlineStr"/>
       <c r="N86" t="inlineStr"/>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>14/03/2017 11:07</t>
-        </is>
-      </c>
+      <c r="O86" t="inlineStr"/>
       <c r="P86" t="inlineStr"/>
       <c r="Q86" t="inlineStr"/>
       <c r="R86" t="inlineStr"/>
@@ -5296,11 +4956,7 @@
       </c>
       <c r="M87" t="inlineStr"/>
       <c r="N87" t="inlineStr"/>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>05/11/2015 15:54</t>
-        </is>
-      </c>
+      <c r="O87" t="inlineStr"/>
       <c r="P87" t="inlineStr"/>
       <c r="Q87" t="inlineStr"/>
       <c r="R87" t="inlineStr"/>
@@ -5353,11 +5009,7 @@
       </c>
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr"/>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>05/11/2015 15:54</t>
-        </is>
-      </c>
+      <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr"/>
       <c r="Q88" t="inlineStr"/>
       <c r="R88" t="inlineStr"/>
@@ -5410,11 +5062,7 @@
       </c>
       <c r="M89" t="inlineStr"/>
       <c r="N89" t="inlineStr"/>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>29/05/2018 15:19</t>
-        </is>
-      </c>
+      <c r="O89" t="inlineStr"/>
       <c r="P89" t="inlineStr"/>
       <c r="Q89" t="inlineStr"/>
       <c r="R89" t="inlineStr"/>
@@ -5467,11 +5115,7 @@
       </c>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="inlineStr"/>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>29/08/2014 15:55</t>
-        </is>
-      </c>
+      <c r="O90" t="inlineStr"/>
       <c r="P90" t="inlineStr"/>
       <c r="Q90" t="inlineStr"/>
       <c r="R90" t="inlineStr"/>
@@ -5524,11 +5168,7 @@
       </c>
       <c r="M91" t="inlineStr"/>
       <c r="N91" t="inlineStr"/>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>08/08/2012 15:11</t>
-        </is>
-      </c>
+      <c r="O91" t="inlineStr"/>
       <c r="P91" t="inlineStr"/>
       <c r="Q91" t="inlineStr"/>
       <c r="R91" t="inlineStr"/>
@@ -5561,11 +5201,7 @@
       </c>
       <c r="M92" t="inlineStr"/>
       <c r="N92" t="inlineStr"/>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>27/03/2015 10:54</t>
-        </is>
-      </c>
+      <c r="O92" t="inlineStr"/>
       <c r="P92" t="inlineStr"/>
       <c r="Q92" t="inlineStr"/>
       <c r="R92" t="inlineStr"/>
@@ -5602,11 +5238,7 @@
       </c>
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="inlineStr"/>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>21/03/2017 15:29</t>
-        </is>
-      </c>
+      <c r="O93" t="inlineStr"/>
       <c r="P93" t="inlineStr"/>
       <c r="Q93" t="inlineStr"/>
       <c r="R93" t="inlineStr"/>
@@ -5639,11 +5271,7 @@
       </c>
       <c r="M94" t="inlineStr"/>
       <c r="N94" t="inlineStr"/>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>27/02/2015 15:58</t>
-        </is>
-      </c>
+      <c r="O94" t="inlineStr"/>
       <c r="P94" t="inlineStr"/>
       <c r="Q94" t="inlineStr"/>
       <c r="R94" t="inlineStr"/>
@@ -5676,11 +5304,7 @@
       </c>
       <c r="M95" t="inlineStr"/>
       <c r="N95" t="inlineStr"/>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>06/11/2014 10:24</t>
-        </is>
-      </c>
+      <c r="O95" t="inlineStr"/>
       <c r="P95" t="inlineStr"/>
       <c r="Q95" t="inlineStr"/>
       <c r="R95" t="inlineStr"/>
@@ -5713,11 +5337,7 @@
       </c>
       <c r="M96" t="inlineStr"/>
       <c r="N96" t="inlineStr"/>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>25/01/2013 10:03</t>
-        </is>
-      </c>
+      <c r="O96" t="inlineStr"/>
       <c r="P96" t="inlineStr"/>
       <c r="Q96" t="inlineStr"/>
       <c r="R96" t="inlineStr"/>
@@ -5750,11 +5370,7 @@
       </c>
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr"/>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>22/05/2014 15:22</t>
-        </is>
-      </c>
+      <c r="O97" t="inlineStr"/>
       <c r="P97" t="inlineStr"/>
       <c r="Q97" t="inlineStr"/>
       <c r="R97" t="inlineStr"/>
@@ -5787,11 +5403,7 @@
       </c>
       <c r="M98" t="inlineStr"/>
       <c r="N98" t="inlineStr"/>
-      <c r="O98" t="inlineStr">
-        <is>
-          <t>14/05/2015 14:20</t>
-        </is>
-      </c>
+      <c r="O98" t="inlineStr"/>
       <c r="P98" t="inlineStr"/>
       <c r="Q98" t="inlineStr"/>
       <c r="R98" t="inlineStr"/>
@@ -5844,11 +5456,7 @@
       </c>
       <c r="M99" t="inlineStr"/>
       <c r="N99" t="inlineStr"/>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>04/02/2016 14:18</t>
-        </is>
-      </c>
+      <c r="O99" t="inlineStr"/>
       <c r="P99" t="inlineStr"/>
       <c r="Q99" t="inlineStr"/>
       <c r="R99" t="inlineStr"/>
@@ -5885,11 +5493,7 @@
       </c>
       <c r="M100" t="inlineStr"/>
       <c r="N100" t="inlineStr"/>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>02/10/2017 15:17</t>
-        </is>
-      </c>
+      <c r="O100" t="inlineStr"/>
       <c r="P100" t="inlineStr"/>
       <c r="Q100" t="inlineStr"/>
       <c r="R100" t="inlineStr"/>
@@ -5946,11 +5550,7 @@
       </c>
       <c r="M101" t="inlineStr"/>
       <c r="N101" t="inlineStr"/>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>04/05/2015 19:57</t>
-        </is>
-      </c>
+      <c r="O101" t="inlineStr"/>
       <c r="P101" t="inlineStr"/>
       <c r="Q101" t="inlineStr"/>
       <c r="R101" t="inlineStr"/>
@@ -6003,11 +5603,7 @@
       </c>
       <c r="M102" t="inlineStr"/>
       <c r="N102" t="inlineStr"/>
-      <c r="O102" t="inlineStr">
-        <is>
-          <t>27/04/2016 18:21</t>
-        </is>
-      </c>
+      <c r="O102" t="inlineStr"/>
       <c r="P102" t="inlineStr"/>
       <c r="Q102" t="inlineStr"/>
       <c r="R102" t="inlineStr"/>
@@ -6060,11 +5656,7 @@
       </c>
       <c r="M103" t="inlineStr"/>
       <c r="N103" t="inlineStr"/>
-      <c r="O103" t="inlineStr">
-        <is>
-          <t>27/07/2021 15:15</t>
-        </is>
-      </c>
+      <c r="O103" t="inlineStr"/>
       <c r="P103" t="inlineStr"/>
       <c r="Q103" t="inlineStr"/>
       <c r="R103" t="inlineStr"/>
@@ -6117,11 +5709,7 @@
       </c>
       <c r="M104" t="inlineStr"/>
       <c r="N104" t="inlineStr"/>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>24/04/2014 13:20</t>
-        </is>
-      </c>
+      <c r="O104" t="inlineStr"/>
       <c r="P104" t="inlineStr"/>
       <c r="Q104" t="inlineStr"/>
       <c r="R104" t="inlineStr"/>
@@ -6170,11 +5758,7 @@
       </c>
       <c r="M105" t="inlineStr"/>
       <c r="N105" t="inlineStr"/>
-      <c r="O105" t="inlineStr">
-        <is>
-          <t>22/02/2013 17:14</t>
-        </is>
-      </c>
+      <c r="O105" t="inlineStr"/>
       <c r="P105" t="inlineStr"/>
       <c r="Q105" t="inlineStr"/>
       <c r="R105" t="inlineStr"/>
@@ -6227,11 +5811,7 @@
       </c>
       <c r="M106" t="inlineStr"/>
       <c r="N106" t="inlineStr"/>
-      <c r="O106" t="inlineStr">
-        <is>
-          <t>20/10/2016 16:54</t>
-        </is>
-      </c>
+      <c r="O106" t="inlineStr"/>
       <c r="P106" t="inlineStr"/>
       <c r="Q106" t="inlineStr"/>
       <c r="R106" t="inlineStr"/>
@@ -6284,11 +5864,7 @@
       </c>
       <c r="M107" t="inlineStr"/>
       <c r="N107" t="inlineStr"/>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>24/08/2017 09:10</t>
-        </is>
-      </c>
+      <c r="O107" t="inlineStr"/>
       <c r="P107" t="inlineStr"/>
       <c r="Q107" t="inlineStr"/>
       <c r="R107" t="inlineStr"/>
@@ -6341,11 +5917,7 @@
       </c>
       <c r="M108" t="inlineStr"/>
       <c r="N108" t="inlineStr"/>
-      <c r="O108" t="inlineStr">
-        <is>
-          <t>19/11/2014 11:23</t>
-        </is>
-      </c>
+      <c r="O108" t="inlineStr"/>
       <c r="P108" t="inlineStr"/>
       <c r="Q108" t="inlineStr"/>
       <c r="R108" t="inlineStr"/>
@@ -6382,11 +5954,7 @@
       </c>
       <c r="M109" t="inlineStr"/>
       <c r="N109" t="inlineStr"/>
-      <c r="O109" t="inlineStr">
-        <is>
-          <t>11/08/2021 15:46</t>
-        </is>
-      </c>
+      <c r="O109" t="inlineStr"/>
       <c r="P109" t="inlineStr"/>
       <c r="Q109" t="inlineStr"/>
       <c r="R109" t="inlineStr"/>
@@ -6439,11 +6007,7 @@
       </c>
       <c r="M110" t="inlineStr"/>
       <c r="N110" t="inlineStr"/>
-      <c r="O110" t="inlineStr">
-        <is>
-          <t>15/12/2014 14:05</t>
-        </is>
-      </c>
+      <c r="O110" t="inlineStr"/>
       <c r="P110" t="inlineStr"/>
       <c r="Q110" t="inlineStr"/>
       <c r="R110" t="inlineStr"/>
@@ -6496,11 +6060,7 @@
       </c>
       <c r="M111" t="inlineStr"/>
       <c r="N111" t="inlineStr"/>
-      <c r="O111" t="inlineStr">
-        <is>
-          <t>22/02/2019 09:55</t>
-        </is>
-      </c>
+      <c r="O111" t="inlineStr"/>
       <c r="P111" t="inlineStr"/>
       <c r="Q111" t="inlineStr"/>
       <c r="R111" t="inlineStr"/>
@@ -6553,11 +6113,7 @@
       </c>
       <c r="M112" t="inlineStr"/>
       <c r="N112" t="inlineStr"/>
-      <c r="O112" t="inlineStr">
-        <is>
-          <t>13/12/2016 21:55</t>
-        </is>
-      </c>
+      <c r="O112" t="inlineStr"/>
       <c r="P112" t="inlineStr"/>
       <c r="Q112" t="inlineStr"/>
       <c r="R112" t="inlineStr"/>
@@ -6610,11 +6166,7 @@
       </c>
       <c r="M113" t="inlineStr"/>
       <c r="N113" t="inlineStr"/>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>19/12/2013 17:30</t>
-        </is>
-      </c>
+      <c r="O113" t="inlineStr"/>
       <c r="P113" t="inlineStr"/>
       <c r="Q113" t="inlineStr"/>
       <c r="R113" t="inlineStr"/>
@@ -6667,11 +6219,7 @@
       </c>
       <c r="M114" t="inlineStr"/>
       <c r="N114" t="inlineStr"/>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>26/06/2018 14:15</t>
-        </is>
-      </c>
+      <c r="O114" t="inlineStr"/>
       <c r="P114" t="inlineStr"/>
       <c r="Q114" t="inlineStr"/>
       <c r="R114" t="inlineStr"/>
@@ -6724,11 +6272,7 @@
       </c>
       <c r="M115" t="inlineStr"/>
       <c r="N115" t="inlineStr"/>
-      <c r="O115" t="inlineStr">
-        <is>
-          <t>19/07/2017 14:10</t>
-        </is>
-      </c>
+      <c r="O115" t="inlineStr"/>
       <c r="P115" t="inlineStr"/>
       <c r="Q115" t="inlineStr"/>
       <c r="R115" t="inlineStr"/>
@@ -6777,11 +6321,7 @@
       </c>
       <c r="M116" t="inlineStr"/>
       <c r="N116" t="inlineStr"/>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>28/05/2014 17:28</t>
-        </is>
-      </c>
+      <c r="O116" t="inlineStr"/>
       <c r="P116" t="inlineStr"/>
       <c r="Q116" t="inlineStr"/>
       <c r="R116" t="inlineStr"/>
@@ -6834,11 +6374,7 @@
       </c>
       <c r="M117" t="inlineStr"/>
       <c r="N117" t="inlineStr"/>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>09/11/2012 19:05</t>
-        </is>
-      </c>
+      <c r="O117" t="inlineStr"/>
       <c r="P117" t="inlineStr"/>
       <c r="Q117" t="inlineStr"/>
       <c r="R117" t="inlineStr"/>
@@ -6887,11 +6423,7 @@
       </c>
       <c r="M118" t="inlineStr"/>
       <c r="N118" t="inlineStr"/>
-      <c r="O118" t="inlineStr">
-        <is>
-          <t>15/07/2016 16:10</t>
-        </is>
-      </c>
+      <c r="O118" t="inlineStr"/>
       <c r="P118" t="inlineStr"/>
       <c r="Q118" t="inlineStr"/>
       <c r="R118" t="inlineStr"/>
@@ -6944,11 +6476,7 @@
       </c>
       <c r="M119" t="inlineStr"/>
       <c r="N119" t="inlineStr"/>
-      <c r="O119" t="inlineStr">
-        <is>
-          <t>18/07/2016 15:12</t>
-        </is>
-      </c>
+      <c r="O119" t="inlineStr"/>
       <c r="P119" t="inlineStr"/>
       <c r="Q119" t="inlineStr"/>
       <c r="R119" t="inlineStr"/>
@@ -7001,11 +6529,7 @@
       </c>
       <c r="M120" t="inlineStr"/>
       <c r="N120" t="inlineStr"/>
-      <c r="O120" t="inlineStr">
-        <is>
-          <t>26/04/2017 10:46</t>
-        </is>
-      </c>
+      <c r="O120" t="inlineStr"/>
       <c r="P120" t="inlineStr"/>
       <c r="Q120" t="inlineStr"/>
       <c r="R120" t="inlineStr"/>
@@ -7058,11 +6582,7 @@
       </c>
       <c r="M121" t="inlineStr"/>
       <c r="N121" t="inlineStr"/>
-      <c r="O121" t="inlineStr">
-        <is>
-          <t>28/01/2018 20:59</t>
-        </is>
-      </c>
+      <c r="O121" t="inlineStr"/>
       <c r="P121" t="inlineStr"/>
       <c r="Q121" t="inlineStr"/>
       <c r="R121" t="inlineStr"/>
@@ -7115,11 +6635,7 @@
       </c>
       <c r="M122" t="inlineStr"/>
       <c r="N122" t="inlineStr"/>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>10/07/2018 16:28</t>
-        </is>
-      </c>
+      <c r="O122" t="inlineStr"/>
       <c r="P122" t="inlineStr"/>
       <c r="Q122" t="inlineStr"/>
       <c r="R122" t="inlineStr"/>
@@ -7168,11 +6684,7 @@
       </c>
       <c r="M123" t="inlineStr"/>
       <c r="N123" t="inlineStr"/>
-      <c r="O123" t="inlineStr">
-        <is>
-          <t>12/09/2018 17:45</t>
-        </is>
-      </c>
+      <c r="O123" t="inlineStr"/>
       <c r="P123" t="inlineStr"/>
       <c r="Q123" t="inlineStr"/>
       <c r="R123" t="inlineStr"/>
@@ -7221,11 +6733,7 @@
       </c>
       <c r="M124" t="inlineStr"/>
       <c r="N124" t="inlineStr"/>
-      <c r="O124" t="inlineStr">
-        <is>
-          <t>20/05/2021 13:31</t>
-        </is>
-      </c>
+      <c r="O124" t="inlineStr"/>
       <c r="P124" t="inlineStr"/>
       <c r="Q124" t="inlineStr"/>
       <c r="R124" t="inlineStr"/>
@@ -7274,11 +6782,7 @@
       </c>
       <c r="M125" t="inlineStr"/>
       <c r="N125" t="inlineStr"/>
-      <c r="O125" t="inlineStr">
-        <is>
-          <t>05/12/2013 15:05</t>
-        </is>
-      </c>
+      <c r="O125" t="inlineStr"/>
       <c r="P125" t="inlineStr"/>
       <c r="Q125" t="inlineStr"/>
       <c r="R125" t="inlineStr"/>
@@ -7331,11 +6835,7 @@
       </c>
       <c r="M126" t="inlineStr"/>
       <c r="N126" t="inlineStr"/>
-      <c r="O126" t="inlineStr">
-        <is>
-          <t>27/08/2019 14:52</t>
-        </is>
-      </c>
+      <c r="O126" t="inlineStr"/>
       <c r="P126" t="inlineStr"/>
       <c r="Q126" t="inlineStr"/>
       <c r="R126" t="inlineStr"/>
@@ -7384,11 +6884,7 @@
       </c>
       <c r="M127" t="inlineStr"/>
       <c r="N127" t="inlineStr"/>
-      <c r="O127" t="inlineStr">
-        <is>
-          <t>11/10/2012 18:40</t>
-        </is>
-      </c>
+      <c r="O127" t="inlineStr"/>
       <c r="P127" t="inlineStr"/>
       <c r="Q127" t="inlineStr"/>
       <c r="R127" t="inlineStr"/>
@@ -7441,11 +6937,7 @@
       </c>
       <c r="M128" t="inlineStr"/>
       <c r="N128" t="inlineStr"/>
-      <c r="O128" t="inlineStr">
-        <is>
-          <t>20/05/2015 14:10</t>
-        </is>
-      </c>
+      <c r="O128" t="inlineStr"/>
       <c r="P128" t="inlineStr"/>
       <c r="Q128" t="inlineStr"/>
       <c r="R128" t="inlineStr"/>
@@ -7478,11 +6970,7 @@
       </c>
       <c r="M129" t="inlineStr"/>
       <c r="N129" t="inlineStr"/>
-      <c r="O129" t="inlineStr">
-        <is>
-          <t>05/04/2019 13:52</t>
-        </is>
-      </c>
+      <c r="O129" t="inlineStr"/>
       <c r="P129" t="inlineStr"/>
       <c r="Q129" t="inlineStr"/>
       <c r="R129" t="inlineStr"/>
@@ -7535,11 +7023,7 @@
       </c>
       <c r="M130" t="inlineStr"/>
       <c r="N130" t="inlineStr"/>
-      <c r="O130" t="inlineStr">
-        <is>
-          <t>18/12/2014 10:24</t>
-        </is>
-      </c>
+      <c r="O130" t="inlineStr"/>
       <c r="P130" t="inlineStr"/>
       <c r="Q130" t="inlineStr"/>
       <c r="R130" t="inlineStr"/>
@@ -7576,11 +7060,7 @@
       </c>
       <c r="M131" t="inlineStr"/>
       <c r="N131" t="inlineStr"/>
-      <c r="O131" t="inlineStr">
-        <is>
-          <t>26/05/2021 14:45</t>
-        </is>
-      </c>
+      <c r="O131" t="inlineStr"/>
       <c r="P131" t="inlineStr"/>
       <c r="Q131" t="inlineStr"/>
       <c r="R131" t="inlineStr"/>
@@ -7629,11 +7109,7 @@
       </c>
       <c r="M132" t="inlineStr"/>
       <c r="N132" t="inlineStr"/>
-      <c r="O132" t="inlineStr">
-        <is>
-          <t>02/03/2018 11:03</t>
-        </is>
-      </c>
+      <c r="O132" t="inlineStr"/>
       <c r="P132" t="inlineStr"/>
       <c r="Q132" t="inlineStr"/>
       <c r="R132" t="inlineStr"/>
@@ -7666,11 +7142,7 @@
       </c>
       <c r="M133" t="inlineStr"/>
       <c r="N133" t="inlineStr"/>
-      <c r="O133" t="inlineStr">
-        <is>
-          <t>11/11/2019 15:04</t>
-        </is>
-      </c>
+      <c r="O133" t="inlineStr"/>
       <c r="P133" t="inlineStr"/>
       <c r="Q133" t="inlineStr"/>
       <c r="R133" t="inlineStr"/>
@@ -7723,11 +7195,7 @@
       </c>
       <c r="M134" t="inlineStr"/>
       <c r="N134" t="inlineStr"/>
-      <c r="O134" t="inlineStr">
-        <is>
-          <t>14/07/2016 10:08</t>
-        </is>
-      </c>
+      <c r="O134" t="inlineStr"/>
       <c r="P134" t="inlineStr"/>
       <c r="Q134" t="inlineStr"/>
       <c r="R134" t="inlineStr"/>
@@ -7780,11 +7248,7 @@
       </c>
       <c r="M135" t="inlineStr"/>
       <c r="N135" t="inlineStr"/>
-      <c r="O135" t="inlineStr">
-        <is>
-          <t>29/12/2015 10:25</t>
-        </is>
-      </c>
+      <c r="O135" t="inlineStr"/>
       <c r="P135" t="inlineStr"/>
       <c r="Q135" t="inlineStr"/>
       <c r="R135" t="inlineStr"/>
@@ -7837,11 +7301,7 @@
       </c>
       <c r="M136" t="inlineStr"/>
       <c r="N136" t="inlineStr"/>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>03/05/2017 11:33</t>
-        </is>
-      </c>
+      <c r="O136" t="inlineStr"/>
       <c r="P136" t="inlineStr"/>
       <c r="Q136" t="inlineStr"/>
       <c r="R136" t="inlineStr"/>
@@ -7894,11 +7354,7 @@
       </c>
       <c r="M137" t="inlineStr"/>
       <c r="N137" t="inlineStr"/>
-      <c r="O137" t="inlineStr">
-        <is>
-          <t>02/10/2018 14:51</t>
-        </is>
-      </c>
+      <c r="O137" t="inlineStr"/>
       <c r="P137" t="inlineStr"/>
       <c r="Q137" t="inlineStr"/>
       <c r="R137" t="inlineStr"/>
@@ -7951,11 +7407,7 @@
       </c>
       <c r="M138" t="inlineStr"/>
       <c r="N138" t="inlineStr"/>
-      <c r="O138" t="inlineStr">
-        <is>
-          <t>24/02/2015 10:19</t>
-        </is>
-      </c>
+      <c r="O138" t="inlineStr"/>
       <c r="P138" t="inlineStr"/>
       <c r="Q138" t="inlineStr"/>
       <c r="R138" t="inlineStr"/>
@@ -8008,11 +7460,7 @@
       </c>
       <c r="M139" t="inlineStr"/>
       <c r="N139" t="inlineStr"/>
-      <c r="O139" t="inlineStr">
-        <is>
-          <t>07/02/2019 16:59</t>
-        </is>
-      </c>
+      <c r="O139" t="inlineStr"/>
       <c r="P139" t="inlineStr"/>
       <c r="Q139" t="inlineStr"/>
       <c r="R139" t="inlineStr"/>
@@ -8065,11 +7513,7 @@
       </c>
       <c r="M140" t="inlineStr"/>
       <c r="N140" t="inlineStr"/>
-      <c r="O140" t="inlineStr">
-        <is>
-          <t>12/02/2020 10:49</t>
-        </is>
-      </c>
+      <c r="O140" t="inlineStr"/>
       <c r="P140" t="inlineStr"/>
       <c r="Q140" t="inlineStr"/>
       <c r="R140" t="inlineStr"/>
@@ -8122,11 +7566,7 @@
       </c>
       <c r="M141" t="inlineStr"/>
       <c r="N141" t="inlineStr"/>
-      <c r="O141" t="inlineStr">
-        <is>
-          <t>08/02/2014 14:54</t>
-        </is>
-      </c>
+      <c r="O141" t="inlineStr"/>
       <c r="P141" t="inlineStr"/>
       <c r="Q141" t="inlineStr"/>
       <c r="R141" t="inlineStr"/>
@@ -8179,11 +7619,7 @@
       </c>
       <c r="M142" t="inlineStr"/>
       <c r="N142" t="inlineStr"/>
-      <c r="O142" t="inlineStr">
-        <is>
-          <t>18/10/2017 16:40</t>
-        </is>
-      </c>
+      <c r="O142" t="inlineStr"/>
       <c r="P142" t="inlineStr"/>
       <c r="Q142" t="inlineStr"/>
       <c r="R142" t="inlineStr"/>
@@ -8220,11 +7656,7 @@
       </c>
       <c r="M143" t="inlineStr"/>
       <c r="N143" t="inlineStr"/>
-      <c r="O143" t="inlineStr">
-        <is>
-          <t>24/11/2021 18:35</t>
-        </is>
-      </c>
+      <c r="O143" t="inlineStr"/>
       <c r="P143" t="inlineStr"/>
       <c r="Q143" t="inlineStr"/>
       <c r="R143" t="inlineStr"/>
@@ -8277,11 +7709,7 @@
       </c>
       <c r="M144" t="inlineStr"/>
       <c r="N144" t="inlineStr"/>
-      <c r="O144" t="inlineStr">
-        <is>
-          <t>07/02/2019 17:33</t>
-        </is>
-      </c>
+      <c r="O144" t="inlineStr"/>
       <c r="P144" t="inlineStr"/>
       <c r="Q144" t="inlineStr"/>
       <c r="R144" t="inlineStr"/>
@@ -8318,11 +7746,7 @@
       </c>
       <c r="M145" t="inlineStr"/>
       <c r="N145" t="inlineStr"/>
-      <c r="O145" t="inlineStr">
-        <is>
-          <t>19/01/2022 14:30</t>
-        </is>
-      </c>
+      <c r="O145" t="inlineStr"/>
       <c r="P145" t="inlineStr"/>
       <c r="Q145" t="inlineStr"/>
       <c r="R145" t="inlineStr"/>
@@ -8379,11 +7803,7 @@
       </c>
       <c r="M146" t="inlineStr"/>
       <c r="N146" t="inlineStr"/>
-      <c r="O146" t="inlineStr">
-        <is>
-          <t>08/08/2012 16:00</t>
-        </is>
-      </c>
+      <c r="O146" t="inlineStr"/>
       <c r="P146" t="inlineStr"/>
       <c r="Q146" t="inlineStr"/>
       <c r="R146" t="inlineStr"/>
@@ -8436,11 +7856,7 @@
       </c>
       <c r="M147" t="inlineStr"/>
       <c r="N147" t="inlineStr"/>
-      <c r="O147" t="inlineStr">
-        <is>
-          <t>09/05/2018 16:31</t>
-        </is>
-      </c>
+      <c r="O147" t="inlineStr"/>
       <c r="P147" t="inlineStr"/>
       <c r="Q147" t="inlineStr"/>
       <c r="R147" t="inlineStr"/>
@@ -8493,11 +7909,7 @@
       </c>
       <c r="M148" t="inlineStr"/>
       <c r="N148" t="inlineStr"/>
-      <c r="O148" t="inlineStr">
-        <is>
-          <t>22/07/2016 10:32</t>
-        </is>
-      </c>
+      <c r="O148" t="inlineStr"/>
       <c r="P148" t="inlineStr"/>
       <c r="Q148" t="inlineStr"/>
       <c r="R148" t="inlineStr"/>
@@ -8550,11 +7962,7 @@
       </c>
       <c r="M149" t="inlineStr"/>
       <c r="N149" t="inlineStr"/>
-      <c r="O149" t="inlineStr">
-        <is>
-          <t>10/10/2017 13:50</t>
-        </is>
-      </c>
+      <c r="O149" t="inlineStr"/>
       <c r="P149" t="inlineStr"/>
       <c r="Q149" t="inlineStr"/>
       <c r="R149" t="inlineStr"/>
@@ -8607,11 +8015,7 @@
       </c>
       <c r="M150" t="inlineStr"/>
       <c r="N150" t="inlineStr"/>
-      <c r="O150" t="inlineStr">
-        <is>
-          <t>14/03/2017 13:43</t>
-        </is>
-      </c>
+      <c r="O150" t="inlineStr"/>
       <c r="P150" t="inlineStr"/>
       <c r="Q150" t="inlineStr"/>
       <c r="R150" t="inlineStr"/>
@@ -8664,11 +8068,7 @@
       </c>
       <c r="M151" t="inlineStr"/>
       <c r="N151" t="inlineStr"/>
-      <c r="O151" t="inlineStr">
-        <is>
-          <t>30/06/2016 16:55</t>
-        </is>
-      </c>
+      <c r="O151" t="inlineStr"/>
       <c r="P151" t="inlineStr"/>
       <c r="Q151" t="inlineStr"/>
       <c r="R151" t="inlineStr"/>
@@ -8721,11 +8121,7 @@
       </c>
       <c r="M152" t="inlineStr"/>
       <c r="N152" t="inlineStr"/>
-      <c r="O152" t="inlineStr">
-        <is>
-          <t>14/07/2016 10:49</t>
-        </is>
-      </c>
+      <c r="O152" t="inlineStr"/>
       <c r="P152" t="inlineStr"/>
       <c r="Q152" t="inlineStr"/>
       <c r="R152" t="inlineStr"/>
@@ -8778,11 +8174,7 @@
       </c>
       <c r="M153" t="inlineStr"/>
       <c r="N153" t="inlineStr"/>
-      <c r="O153" t="inlineStr">
-        <is>
-          <t>12/01/2018 09:31</t>
-        </is>
-      </c>
+      <c r="O153" t="inlineStr"/>
       <c r="P153" t="inlineStr"/>
       <c r="Q153" t="inlineStr"/>
       <c r="R153" t="inlineStr"/>
@@ -8835,11 +8227,7 @@
       </c>
       <c r="M154" t="inlineStr"/>
       <c r="N154" t="inlineStr"/>
-      <c r="O154" t="inlineStr">
-        <is>
-          <t>05/07/2017 10:49</t>
-        </is>
-      </c>
+      <c r="O154" t="inlineStr"/>
       <c r="P154" t="inlineStr"/>
       <c r="Q154" t="inlineStr"/>
       <c r="R154" t="inlineStr"/>
@@ -8892,11 +8280,7 @@
       </c>
       <c r="M155" t="inlineStr"/>
       <c r="N155" t="inlineStr"/>
-      <c r="O155" t="inlineStr">
-        <is>
-          <t>26/10/2017 10:01</t>
-        </is>
-      </c>
+      <c r="O155" t="inlineStr"/>
       <c r="P155" t="inlineStr"/>
       <c r="Q155" t="inlineStr"/>
       <c r="R155" t="inlineStr"/>
@@ -8949,11 +8333,7 @@
       </c>
       <c r="M156" t="inlineStr"/>
       <c r="N156" t="inlineStr"/>
-      <c r="O156" t="inlineStr">
-        <is>
-          <t>04/04/2017 16:41</t>
-        </is>
-      </c>
+      <c r="O156" t="inlineStr"/>
       <c r="P156" t="inlineStr"/>
       <c r="Q156" t="inlineStr"/>
       <c r="R156" t="inlineStr"/>
@@ -9006,11 +8386,7 @@
       </c>
       <c r="M157" t="inlineStr"/>
       <c r="N157" t="inlineStr"/>
-      <c r="O157" t="inlineStr">
-        <is>
-          <t>27/01/2021 09:45</t>
-        </is>
-      </c>
+      <c r="O157" t="inlineStr"/>
       <c r="P157" t="inlineStr"/>
       <c r="Q157" t="inlineStr"/>
       <c r="R157" t="inlineStr"/>
@@ -9063,11 +8439,7 @@
       </c>
       <c r="M158" t="inlineStr"/>
       <c r="N158" t="inlineStr"/>
-      <c r="O158" t="inlineStr">
-        <is>
-          <t>20/11/2018 14:45</t>
-        </is>
-      </c>
+      <c r="O158" t="inlineStr"/>
       <c r="P158" t="inlineStr"/>
       <c r="Q158" t="inlineStr"/>
       <c r="R158" t="inlineStr"/>
@@ -9120,11 +8492,7 @@
       </c>
       <c r="M159" t="inlineStr"/>
       <c r="N159" t="inlineStr"/>
-      <c r="O159" t="inlineStr">
-        <is>
-          <t>07/06/2018 19:05</t>
-        </is>
-      </c>
+      <c r="O159" t="inlineStr"/>
       <c r="P159" t="inlineStr"/>
       <c r="Q159" t="inlineStr"/>
       <c r="R159" t="inlineStr"/>
@@ -9177,11 +8545,7 @@
       </c>
       <c r="M160" t="inlineStr"/>
       <c r="N160" t="inlineStr"/>
-      <c r="O160" t="inlineStr">
-        <is>
-          <t>27/10/2017 14:17</t>
-        </is>
-      </c>
+      <c r="O160" t="inlineStr"/>
       <c r="P160" t="inlineStr"/>
       <c r="Q160" t="inlineStr"/>
       <c r="R160" t="inlineStr"/>
@@ -9234,11 +8598,7 @@
       </c>
       <c r="M161" t="inlineStr"/>
       <c r="N161" t="inlineStr"/>
-      <c r="O161" t="inlineStr">
-        <is>
-          <t>01/11/2017 15:01</t>
-        </is>
-      </c>
+      <c r="O161" t="inlineStr"/>
       <c r="P161" t="inlineStr"/>
       <c r="Q161" t="inlineStr"/>
       <c r="R161" t="inlineStr"/>
@@ -9291,11 +8651,7 @@
       </c>
       <c r="M162" t="inlineStr"/>
       <c r="N162" t="inlineStr"/>
-      <c r="O162" t="inlineStr">
-        <is>
-          <t>18/09/2014 10:53</t>
-        </is>
-      </c>
+      <c r="O162" t="inlineStr"/>
       <c r="P162" t="inlineStr"/>
       <c r="Q162" t="inlineStr"/>
       <c r="R162" t="inlineStr"/>
@@ -9348,11 +8704,7 @@
       </c>
       <c r="M163" t="inlineStr"/>
       <c r="N163" t="inlineStr"/>
-      <c r="O163" t="inlineStr">
-        <is>
-          <t>01/12/2016 17:50</t>
-        </is>
-      </c>
+      <c r="O163" t="inlineStr"/>
       <c r="P163" t="inlineStr"/>
       <c r="Q163" t="inlineStr"/>
       <c r="R163" t="inlineStr"/>
@@ -9405,11 +8757,7 @@
       </c>
       <c r="M164" t="inlineStr"/>
       <c r="N164" t="inlineStr"/>
-      <c r="O164" t="inlineStr">
-        <is>
-          <t>06/06/2018 10:39</t>
-        </is>
-      </c>
+      <c r="O164" t="inlineStr"/>
       <c r="P164" t="inlineStr"/>
       <c r="Q164" t="inlineStr"/>
       <c r="R164" t="inlineStr"/>
@@ -9462,11 +8810,7 @@
       </c>
       <c r="M165" t="inlineStr"/>
       <c r="N165" t="inlineStr"/>
-      <c r="O165" t="inlineStr">
-        <is>
-          <t>31/08/2012 17:26</t>
-        </is>
-      </c>
+      <c r="O165" t="inlineStr"/>
       <c r="P165" t="inlineStr"/>
       <c r="Q165" t="inlineStr"/>
       <c r="R165" t="inlineStr"/>
@@ -9519,11 +8863,7 @@
       </c>
       <c r="M166" t="inlineStr"/>
       <c r="N166" t="inlineStr"/>
-      <c r="O166" t="inlineStr">
-        <is>
-          <t>20/11/2017 17:54</t>
-        </is>
-      </c>
+      <c r="O166" t="inlineStr"/>
       <c r="P166" t="inlineStr"/>
       <c r="Q166" t="inlineStr"/>
       <c r="R166" t="inlineStr"/>
@@ -9576,11 +8916,7 @@
       </c>
       <c r="M167" t="inlineStr"/>
       <c r="N167" t="inlineStr"/>
-      <c r="O167" t="inlineStr">
-        <is>
-          <t>01/02/2013 14:00</t>
-        </is>
-      </c>
+      <c r="O167" t="inlineStr"/>
       <c r="P167" t="inlineStr"/>
       <c r="Q167" t="inlineStr"/>
       <c r="R167" t="inlineStr"/>
@@ -9633,11 +8969,7 @@
       </c>
       <c r="M168" t="inlineStr"/>
       <c r="N168" t="inlineStr"/>
-      <c r="O168" t="inlineStr">
-        <is>
-          <t>15/07/2016 15:44</t>
-        </is>
-      </c>
+      <c r="O168" t="inlineStr"/>
       <c r="P168" t="inlineStr"/>
       <c r="Q168" t="inlineStr"/>
       <c r="R168" t="inlineStr"/>
@@ -9690,11 +9022,7 @@
       </c>
       <c r="M169" t="inlineStr"/>
       <c r="N169" t="inlineStr"/>
-      <c r="O169" t="inlineStr">
-        <is>
-          <t>13/01/2020 11:29</t>
-        </is>
-      </c>
+      <c r="O169" t="inlineStr"/>
       <c r="P169" t="inlineStr"/>
       <c r="Q169" t="inlineStr"/>
       <c r="R169" t="inlineStr"/>
@@ -9747,11 +9075,7 @@
       </c>
       <c r="M170" t="inlineStr"/>
       <c r="N170" t="inlineStr"/>
-      <c r="O170" t="inlineStr">
-        <is>
-          <t>04/08/2016 16:41</t>
-        </is>
-      </c>
+      <c r="O170" t="inlineStr"/>
       <c r="P170" t="inlineStr"/>
       <c r="Q170" t="inlineStr"/>
       <c r="R170" t="inlineStr"/>
@@ -9804,11 +9128,7 @@
       </c>
       <c r="M171" t="inlineStr"/>
       <c r="N171" t="inlineStr"/>
-      <c r="O171" t="inlineStr">
-        <is>
-          <t>08/10/2020 14:22</t>
-        </is>
-      </c>
+      <c r="O171" t="inlineStr"/>
       <c r="P171" t="inlineStr"/>
       <c r="Q171" t="inlineStr"/>
       <c r="R171" t="inlineStr"/>
@@ -9865,11 +9185,7 @@
       </c>
       <c r="M172" t="inlineStr"/>
       <c r="N172" t="inlineStr"/>
-      <c r="O172" t="inlineStr">
-        <is>
-          <t>19/09/2012 14:36</t>
-        </is>
-      </c>
+      <c r="O172" t="inlineStr"/>
       <c r="P172" t="inlineStr"/>
       <c r="Q172" t="inlineStr"/>
       <c r="R172" t="inlineStr"/>
@@ -9922,11 +9238,7 @@
       </c>
       <c r="M173" t="inlineStr"/>
       <c r="N173" t="inlineStr"/>
-      <c r="O173" t="inlineStr">
-        <is>
-          <t>23/02/2017 15:37</t>
-        </is>
-      </c>
+      <c r="O173" t="inlineStr"/>
       <c r="P173" t="inlineStr"/>
       <c r="Q173" t="inlineStr"/>
       <c r="R173" t="inlineStr"/>
@@ -9979,11 +9291,7 @@
       </c>
       <c r="M174" t="inlineStr"/>
       <c r="N174" t="inlineStr"/>
-      <c r="O174" t="inlineStr">
-        <is>
-          <t>03/07/2017 10:58</t>
-        </is>
-      </c>
+      <c r="O174" t="inlineStr"/>
       <c r="P174" t="inlineStr"/>
       <c r="Q174" t="inlineStr"/>
       <c r="R174" t="inlineStr"/>
@@ -10024,11 +9332,7 @@
       </c>
       <c r="M175" t="inlineStr"/>
       <c r="N175" t="inlineStr"/>
-      <c r="O175" t="inlineStr">
-        <is>
-          <t>01/04/2021 12:40</t>
-        </is>
-      </c>
+      <c r="O175" t="inlineStr"/>
       <c r="P175" t="inlineStr"/>
       <c r="Q175" t="inlineStr"/>
       <c r="R175" t="inlineStr"/>
@@ -10081,11 +9385,7 @@
       </c>
       <c r="M176" t="inlineStr"/>
       <c r="N176" t="inlineStr"/>
-      <c r="O176" t="inlineStr">
-        <is>
-          <t>22/08/2019 11:39</t>
-        </is>
-      </c>
+      <c r="O176" t="inlineStr"/>
       <c r="P176" t="inlineStr"/>
       <c r="Q176" t="inlineStr"/>
       <c r="R176" t="inlineStr"/>
@@ -10138,11 +9438,7 @@
       </c>
       <c r="M177" t="inlineStr"/>
       <c r="N177" t="inlineStr"/>
-      <c r="O177" t="inlineStr">
-        <is>
-          <t>07/11/2019 17:55</t>
-        </is>
-      </c>
+      <c r="O177" t="inlineStr"/>
       <c r="P177" t="inlineStr"/>
       <c r="Q177" t="inlineStr"/>
       <c r="R177" t="inlineStr"/>
@@ -10191,11 +9487,7 @@
       </c>
       <c r="M178" t="inlineStr"/>
       <c r="N178" t="inlineStr"/>
-      <c r="O178" t="inlineStr">
-        <is>
-          <t>11/02/2019 18:19</t>
-        </is>
-      </c>
+      <c r="O178" t="inlineStr"/>
       <c r="P178" t="inlineStr"/>
       <c r="Q178" t="inlineStr"/>
       <c r="R178" t="inlineStr"/>
@@ -10244,16 +9536,8 @@
       </c>
       <c r="M179" t="inlineStr"/>
       <c r="N179" t="inlineStr"/>
-      <c r="O179" t="inlineStr">
-        <is>
-          <t>22/11/2012 08:53</t>
-        </is>
-      </c>
-      <c r="P179" t="inlineStr">
-        <is>
-          <t>22/11/2012 00:00</t>
-        </is>
-      </c>
+      <c r="O179" t="inlineStr"/>
+      <c r="P179" t="inlineStr"/>
       <c r="Q179" t="inlineStr"/>
       <c r="R179" t="inlineStr"/>
       <c r="S179" t="inlineStr"/>
@@ -10289,11 +9573,7 @@
       </c>
       <c r="M180" t="inlineStr"/>
       <c r="N180" t="inlineStr"/>
-      <c r="O180" t="inlineStr">
-        <is>
-          <t>24/04/2019 10:52</t>
-        </is>
-      </c>
+      <c r="O180" t="inlineStr"/>
       <c r="P180" t="inlineStr"/>
       <c r="Q180" t="inlineStr"/>
       <c r="R180" t="inlineStr"/>
@@ -10346,11 +9626,7 @@
       </c>
       <c r="M181" t="inlineStr"/>
       <c r="N181" t="inlineStr"/>
-      <c r="O181" t="inlineStr">
-        <is>
-          <t>21/08/2017 10:45</t>
-        </is>
-      </c>
+      <c r="O181" t="inlineStr"/>
       <c r="P181" t="inlineStr"/>
       <c r="Q181" t="inlineStr"/>
       <c r="R181" t="inlineStr"/>
@@ -10403,11 +9679,7 @@
       </c>
       <c r="M182" t="inlineStr"/>
       <c r="N182" t="inlineStr"/>
-      <c r="O182" t="inlineStr">
-        <is>
-          <t>01/09/2014 14:27</t>
-        </is>
-      </c>
+      <c r="O182" t="inlineStr"/>
       <c r="P182" t="inlineStr"/>
       <c r="Q182" t="inlineStr"/>
       <c r="R182" t="inlineStr"/>
@@ -10460,11 +9732,7 @@
       </c>
       <c r="M183" t="inlineStr"/>
       <c r="N183" t="inlineStr"/>
-      <c r="O183" t="inlineStr">
-        <is>
-          <t>14/05/2015 16:21</t>
-        </is>
-      </c>
+      <c r="O183" t="inlineStr"/>
       <c r="P183" t="inlineStr"/>
       <c r="Q183" t="inlineStr"/>
       <c r="R183" t="inlineStr"/>
@@ -10517,11 +9785,7 @@
       </c>
       <c r="M184" t="inlineStr"/>
       <c r="N184" t="inlineStr"/>
-      <c r="O184" t="inlineStr">
-        <is>
-          <t>16/07/2015 10:00</t>
-        </is>
-      </c>
+      <c r="O184" t="inlineStr"/>
       <c r="P184" t="inlineStr"/>
       <c r="Q184" t="inlineStr"/>
       <c r="R184" t="inlineStr"/>
@@ -10574,11 +9838,7 @@
       </c>
       <c r="M185" t="inlineStr"/>
       <c r="N185" t="inlineStr"/>
-      <c r="O185" t="inlineStr">
-        <is>
-          <t>07/08/2014 11:13</t>
-        </is>
-      </c>
+      <c r="O185" t="inlineStr"/>
       <c r="P185" t="inlineStr"/>
       <c r="Q185" t="inlineStr"/>
       <c r="R185" t="inlineStr"/>
@@ -10631,11 +9891,7 @@
       </c>
       <c r="M186" t="inlineStr"/>
       <c r="N186" t="inlineStr"/>
-      <c r="O186" t="inlineStr">
-        <is>
-          <t>07/08/2014 11:13</t>
-        </is>
-      </c>
+      <c r="O186" t="inlineStr"/>
       <c r="P186" t="inlineStr"/>
       <c r="Q186" t="inlineStr"/>
       <c r="R186" t="inlineStr"/>
@@ -10688,11 +9944,7 @@
       </c>
       <c r="M187" t="inlineStr"/>
       <c r="N187" t="inlineStr"/>
-      <c r="O187" t="inlineStr">
-        <is>
-          <t>31/05/2017 15:51</t>
-        </is>
-      </c>
+      <c r="O187" t="inlineStr"/>
       <c r="P187" t="inlineStr"/>
       <c r="Q187" t="inlineStr"/>
       <c r="R187" t="inlineStr"/>
@@ -10745,11 +9997,7 @@
       </c>
       <c r="M188" t="inlineStr"/>
       <c r="N188" t="inlineStr"/>
-      <c r="O188" t="inlineStr">
-        <is>
-          <t>08/06/2018 16:03</t>
-        </is>
-      </c>
+      <c r="O188" t="inlineStr"/>
       <c r="P188" t="inlineStr"/>
       <c r="Q188" t="inlineStr"/>
       <c r="R188" t="inlineStr"/>
@@ -10798,11 +10046,7 @@
       </c>
       <c r="M189" t="inlineStr"/>
       <c r="N189" t="inlineStr"/>
-      <c r="O189" t="inlineStr">
-        <is>
-          <t>24/08/2012 17:55</t>
-        </is>
-      </c>
+      <c r="O189" t="inlineStr"/>
       <c r="P189" t="inlineStr"/>
       <c r="Q189" t="inlineStr"/>
       <c r="R189" t="inlineStr"/>
@@ -10855,11 +10099,7 @@
       </c>
       <c r="M190" t="inlineStr"/>
       <c r="N190" t="inlineStr"/>
-      <c r="O190" t="inlineStr">
-        <is>
-          <t>28/08/2014 10:07</t>
-        </is>
-      </c>
+      <c r="O190" t="inlineStr"/>
       <c r="P190" t="inlineStr"/>
       <c r="Q190" t="inlineStr"/>
       <c r="R190" t="inlineStr"/>
@@ -10896,11 +10136,7 @@
       </c>
       <c r="M191" t="inlineStr"/>
       <c r="N191" t="inlineStr"/>
-      <c r="O191" t="inlineStr">
-        <is>
-          <t>05/12/2019 17:09</t>
-        </is>
-      </c>
+      <c r="O191" t="inlineStr"/>
       <c r="P191" t="inlineStr"/>
       <c r="Q191" t="inlineStr"/>
       <c r="R191" t="inlineStr"/>
@@ -10953,11 +10189,7 @@
       </c>
       <c r="M192" t="inlineStr"/>
       <c r="N192" t="inlineStr"/>
-      <c r="O192" t="inlineStr">
-        <is>
-          <t>16/09/2019 16:53</t>
-        </is>
-      </c>
+      <c r="O192" t="inlineStr"/>
       <c r="P192" t="inlineStr"/>
       <c r="Q192" t="inlineStr"/>
       <c r="R192" t="inlineStr"/>
@@ -11010,11 +10242,7 @@
       </c>
       <c r="M193" t="inlineStr"/>
       <c r="N193" t="inlineStr"/>
-      <c r="O193" t="inlineStr">
-        <is>
-          <t>02/07/2019 11:47</t>
-        </is>
-      </c>
+      <c r="O193" t="inlineStr"/>
       <c r="P193" t="inlineStr"/>
       <c r="Q193" t="inlineStr"/>
       <c r="R193" t="inlineStr"/>
@@ -11067,11 +10295,7 @@
       </c>
       <c r="M194" t="inlineStr"/>
       <c r="N194" t="inlineStr"/>
-      <c r="O194" t="inlineStr">
-        <is>
-          <t>31/05/2016 17:12</t>
-        </is>
-      </c>
+      <c r="O194" t="inlineStr"/>
       <c r="P194" t="inlineStr"/>
       <c r="Q194" t="inlineStr"/>
       <c r="R194" t="inlineStr"/>
@@ -11124,11 +10348,7 @@
       </c>
       <c r="M195" t="inlineStr"/>
       <c r="N195" t="inlineStr"/>
-      <c r="O195" t="inlineStr">
-        <is>
-          <t>22/11/2021 14:28</t>
-        </is>
-      </c>
+      <c r="O195" t="inlineStr"/>
       <c r="P195" t="inlineStr"/>
       <c r="Q195" t="inlineStr"/>
       <c r="R195" t="inlineStr"/>
@@ -11181,11 +10401,7 @@
       </c>
       <c r="M196" t="inlineStr"/>
       <c r="N196" t="inlineStr"/>
-      <c r="O196" t="inlineStr">
-        <is>
-          <t>17/07/2018 14:33</t>
-        </is>
-      </c>
+      <c r="O196" t="inlineStr"/>
       <c r="P196" t="inlineStr"/>
       <c r="Q196" t="inlineStr"/>
       <c r="R196" t="inlineStr"/>
@@ -11226,11 +10442,7 @@
       </c>
       <c r="M197" t="inlineStr"/>
       <c r="N197" t="inlineStr"/>
-      <c r="O197" t="inlineStr">
-        <is>
-          <t>09/08/2021 16:03</t>
-        </is>
-      </c>
+      <c r="O197" t="inlineStr"/>
       <c r="P197" t="inlineStr"/>
       <c r="Q197" t="inlineStr"/>
       <c r="R197" t="inlineStr"/>
@@ -11279,11 +10491,7 @@
       </c>
       <c r="M198" t="inlineStr"/>
       <c r="N198" t="inlineStr"/>
-      <c r="O198" t="inlineStr">
-        <is>
-          <t>14/03/2014 10:32</t>
-        </is>
-      </c>
+      <c r="O198" t="inlineStr"/>
       <c r="P198" t="inlineStr"/>
       <c r="Q198" t="inlineStr"/>
       <c r="R198" t="inlineStr"/>
@@ -11336,11 +10544,7 @@
       </c>
       <c r="M199" t="inlineStr"/>
       <c r="N199" t="inlineStr"/>
-      <c r="O199" t="inlineStr">
-        <is>
-          <t>19/04/2013 18:23</t>
-        </is>
-      </c>
+      <c r="O199" t="inlineStr"/>
       <c r="P199" t="inlineStr"/>
       <c r="Q199" t="inlineStr"/>
       <c r="R199" t="inlineStr"/>
@@ -11377,11 +10581,7 @@
       </c>
       <c r="M200" t="inlineStr"/>
       <c r="N200" t="inlineStr"/>
-      <c r="O200" t="inlineStr">
-        <is>
-          <t>15/12/2021 13:58</t>
-        </is>
-      </c>
+      <c r="O200" t="inlineStr"/>
       <c r="P200" t="inlineStr"/>
       <c r="Q200" t="inlineStr"/>
       <c r="R200" t="inlineStr"/>
@@ -11418,11 +10618,7 @@
       </c>
       <c r="M201" t="inlineStr"/>
       <c r="N201" t="inlineStr"/>
-      <c r="O201" t="inlineStr">
-        <is>
-          <t>04/02/2019 12:19</t>
-        </is>
-      </c>
+      <c r="O201" t="inlineStr"/>
       <c r="P201" t="inlineStr"/>
       <c r="Q201" t="inlineStr"/>
       <c r="R201" t="inlineStr"/>
@@ -11471,11 +10667,7 @@
       </c>
       <c r="M202" t="inlineStr"/>
       <c r="N202" t="inlineStr"/>
-      <c r="O202" t="inlineStr">
-        <is>
-          <t>23/08/2013 14:43</t>
-        </is>
-      </c>
+      <c r="O202" t="inlineStr"/>
       <c r="P202" t="inlineStr"/>
       <c r="Q202" t="inlineStr"/>
       <c r="R202" t="inlineStr"/>
@@ -11524,11 +10716,7 @@
       </c>
       <c r="M203" t="inlineStr"/>
       <c r="N203" t="inlineStr"/>
-      <c r="O203" t="inlineStr">
-        <is>
-          <t>17/09/2013 13:57</t>
-        </is>
-      </c>
+      <c r="O203" t="inlineStr"/>
       <c r="P203" t="inlineStr"/>
       <c r="Q203" t="inlineStr"/>
       <c r="R203" t="inlineStr"/>
@@ -11581,11 +10769,7 @@
       </c>
       <c r="M204" t="inlineStr"/>
       <c r="N204" t="inlineStr"/>
-      <c r="O204" t="inlineStr">
-        <is>
-          <t>22/08/2016 14:20</t>
-        </is>
-      </c>
+      <c r="O204" t="inlineStr"/>
       <c r="P204" t="inlineStr"/>
       <c r="Q204" t="inlineStr"/>
       <c r="R204" t="inlineStr"/>
@@ -11638,11 +10822,7 @@
       </c>
       <c r="M205" t="inlineStr"/>
       <c r="N205" t="inlineStr"/>
-      <c r="O205" t="inlineStr">
-        <is>
-          <t>26/01/2016 17:42</t>
-        </is>
-      </c>
+      <c r="O205" t="inlineStr"/>
       <c r="P205" t="inlineStr"/>
       <c r="Q205" t="inlineStr"/>
       <c r="R205" t="inlineStr"/>
@@ -11695,11 +10875,7 @@
       </c>
       <c r="M206" t="inlineStr"/>
       <c r="N206" t="inlineStr"/>
-      <c r="O206" t="inlineStr">
-        <is>
-          <t>05/12/2019 15:58</t>
-        </is>
-      </c>
+      <c r="O206" t="inlineStr"/>
       <c r="P206" t="inlineStr"/>
       <c r="Q206" t="inlineStr"/>
       <c r="R206" t="inlineStr"/>
@@ -11752,11 +10928,7 @@
       </c>
       <c r="M207" t="inlineStr"/>
       <c r="N207" t="inlineStr"/>
-      <c r="O207" t="inlineStr">
-        <is>
-          <t>01/12/2016 15:29</t>
-        </is>
-      </c>
+      <c r="O207" t="inlineStr"/>
       <c r="P207" t="inlineStr"/>
       <c r="Q207" t="inlineStr"/>
       <c r="R207" t="inlineStr"/>
@@ -11809,11 +10981,7 @@
       </c>
       <c r="M208" t="inlineStr"/>
       <c r="N208" t="inlineStr"/>
-      <c r="O208" t="inlineStr">
-        <is>
-          <t>18/01/2017 18:28</t>
-        </is>
-      </c>
+      <c r="O208" t="inlineStr"/>
       <c r="P208" t="inlineStr"/>
       <c r="Q208" t="inlineStr"/>
       <c r="R208" t="inlineStr"/>
@@ -11866,11 +11034,7 @@
       </c>
       <c r="M209" t="inlineStr"/>
       <c r="N209" t="inlineStr"/>
-      <c r="O209" t="inlineStr">
-        <is>
-          <t>05/10/2018 14:31</t>
-        </is>
-      </c>
+      <c r="O209" t="inlineStr"/>
       <c r="P209" t="inlineStr"/>
       <c r="Q209" t="inlineStr"/>
       <c r="R209" t="inlineStr"/>
@@ -11923,11 +11087,7 @@
       </c>
       <c r="M210" t="inlineStr"/>
       <c r="N210" t="inlineStr"/>
-      <c r="O210" t="inlineStr">
-        <is>
-          <t>30/12/2014 16:17</t>
-        </is>
-      </c>
+      <c r="O210" t="inlineStr"/>
       <c r="P210" t="inlineStr"/>
       <c r="Q210" t="inlineStr"/>
       <c r="R210" t="inlineStr"/>
@@ -11980,11 +11140,7 @@
       </c>
       <c r="M211" t="inlineStr"/>
       <c r="N211" t="inlineStr"/>
-      <c r="O211" t="inlineStr">
-        <is>
-          <t>25/05/2015 10:36</t>
-        </is>
-      </c>
+      <c r="O211" t="inlineStr"/>
       <c r="P211" t="inlineStr"/>
       <c r="Q211" t="inlineStr"/>
       <c r="R211" t="inlineStr"/>
@@ -12025,11 +11181,7 @@
       </c>
       <c r="M212" t="inlineStr"/>
       <c r="N212" t="inlineStr"/>
-      <c r="O212" t="inlineStr">
-        <is>
-          <t>28/05/2020 14:28</t>
-        </is>
-      </c>
+      <c r="O212" t="inlineStr"/>
       <c r="P212" t="inlineStr"/>
       <c r="Q212" t="inlineStr"/>
       <c r="R212" t="inlineStr"/>
@@ -12082,11 +11234,7 @@
       </c>
       <c r="M213" t="inlineStr"/>
       <c r="N213" t="inlineStr"/>
-      <c r="O213" t="inlineStr">
-        <is>
-          <t>04/02/2019 16:55</t>
-        </is>
-      </c>
+      <c r="O213" t="inlineStr"/>
       <c r="P213" t="inlineStr"/>
       <c r="Q213" t="inlineStr"/>
       <c r="R213" t="inlineStr"/>
@@ -12139,11 +11287,7 @@
       </c>
       <c r="M214" t="inlineStr"/>
       <c r="N214" t="inlineStr"/>
-      <c r="O214" t="inlineStr">
-        <is>
-          <t>22/11/2021 17:06</t>
-        </is>
-      </c>
+      <c r="O214" t="inlineStr"/>
       <c r="P214" t="inlineStr"/>
       <c r="Q214" t="inlineStr"/>
       <c r="R214" t="inlineStr"/>
@@ -12196,11 +11340,7 @@
       </c>
       <c r="M215" t="inlineStr"/>
       <c r="N215" t="inlineStr"/>
-      <c r="O215" t="inlineStr">
-        <is>
-          <t>26/04/2017 15:36</t>
-        </is>
-      </c>
+      <c r="O215" t="inlineStr"/>
       <c r="P215" t="inlineStr"/>
       <c r="Q215" t="inlineStr"/>
       <c r="R215" t="inlineStr"/>
@@ -12237,11 +11377,7 @@
       </c>
       <c r="M216" t="inlineStr"/>
       <c r="N216" t="inlineStr"/>
-      <c r="O216" t="inlineStr">
-        <is>
-          <t>23/04/2018 13:29</t>
-        </is>
-      </c>
+      <c r="O216" t="inlineStr"/>
       <c r="P216" t="inlineStr"/>
       <c r="Q216" t="inlineStr"/>
       <c r="R216" t="inlineStr"/>
@@ -12294,11 +11430,7 @@
       </c>
       <c r="M217" t="inlineStr"/>
       <c r="N217" t="inlineStr"/>
-      <c r="O217" t="inlineStr">
-        <is>
-          <t>20/11/2019 14:40</t>
-        </is>
-      </c>
+      <c r="O217" t="inlineStr"/>
       <c r="P217" t="inlineStr"/>
       <c r="Q217" t="inlineStr"/>
       <c r="R217" t="inlineStr"/>
@@ -12335,11 +11467,7 @@
       </c>
       <c r="M218" t="inlineStr"/>
       <c r="N218" t="inlineStr"/>
-      <c r="O218" t="inlineStr">
-        <is>
-          <t>03/12/2021 17:13</t>
-        </is>
-      </c>
+      <c r="O218" t="inlineStr"/>
       <c r="P218" t="inlineStr"/>
       <c r="Q218" t="inlineStr"/>
       <c r="R218" t="inlineStr"/>
@@ -12388,11 +11516,7 @@
       </c>
       <c r="M219" t="inlineStr"/>
       <c r="N219" t="inlineStr"/>
-      <c r="O219" t="inlineStr">
-        <is>
-          <t>20/01/2017 16:48</t>
-        </is>
-      </c>
+      <c r="O219" t="inlineStr"/>
       <c r="P219" t="inlineStr"/>
       <c r="Q219" t="inlineStr"/>
       <c r="R219" t="inlineStr"/>
@@ -12445,11 +11569,7 @@
       </c>
       <c r="M220" t="inlineStr"/>
       <c r="N220" t="inlineStr"/>
-      <c r="O220" t="inlineStr">
-        <is>
-          <t>18/10/2017 15:39</t>
-        </is>
-      </c>
+      <c r="O220" t="inlineStr"/>
       <c r="P220" t="inlineStr"/>
       <c r="Q220" t="inlineStr"/>
       <c r="R220" t="inlineStr"/>
@@ -12502,11 +11622,7 @@
       </c>
       <c r="M221" t="inlineStr"/>
       <c r="N221" t="inlineStr"/>
-      <c r="O221" t="inlineStr">
-        <is>
-          <t>11/02/2015 08:42</t>
-        </is>
-      </c>
+      <c r="O221" t="inlineStr"/>
       <c r="P221" t="inlineStr"/>
       <c r="Q221" t="inlineStr"/>
       <c r="R221" t="inlineStr"/>
@@ -12559,11 +11675,7 @@
       </c>
       <c r="M222" t="inlineStr"/>
       <c r="N222" t="inlineStr"/>
-      <c r="O222" t="inlineStr">
-        <is>
-          <t>16/12/2016 08:35</t>
-        </is>
-      </c>
+      <c r="O222" t="inlineStr"/>
       <c r="P222" t="inlineStr"/>
       <c r="Q222" t="inlineStr"/>
       <c r="R222" t="inlineStr"/>
@@ -12600,11 +11712,7 @@
       </c>
       <c r="M223" t="inlineStr"/>
       <c r="N223" t="inlineStr"/>
-      <c r="O223" t="inlineStr">
-        <is>
-          <t>26/05/2021 15:48</t>
-        </is>
-      </c>
+      <c r="O223" t="inlineStr"/>
       <c r="P223" t="inlineStr"/>
       <c r="Q223" t="inlineStr"/>
       <c r="R223" t="inlineStr"/>
@@ -12657,11 +11765,7 @@
       </c>
       <c r="M224" t="inlineStr"/>
       <c r="N224" t="inlineStr"/>
-      <c r="O224" t="inlineStr">
-        <is>
-          <t>03/05/2017 10:48</t>
-        </is>
-      </c>
+      <c r="O224" t="inlineStr"/>
       <c r="P224" t="inlineStr"/>
       <c r="Q224" t="inlineStr"/>
       <c r="R224" t="inlineStr"/>
@@ -12714,11 +11818,7 @@
       </c>
       <c r="M225" t="inlineStr"/>
       <c r="N225" t="inlineStr"/>
-      <c r="O225" t="inlineStr">
-        <is>
-          <t>12/12/2016 14:21</t>
-        </is>
-      </c>
+      <c r="O225" t="inlineStr"/>
       <c r="P225" t="inlineStr"/>
       <c r="Q225" t="inlineStr"/>
       <c r="R225" t="inlineStr"/>
@@ -12771,11 +11871,7 @@
       </c>
       <c r="M226" t="inlineStr"/>
       <c r="N226" t="inlineStr"/>
-      <c r="O226" t="inlineStr">
-        <is>
-          <t>21/09/2017 16:34</t>
-        </is>
-      </c>
+      <c r="O226" t="inlineStr"/>
       <c r="P226" t="inlineStr"/>
       <c r="Q226" t="inlineStr"/>
       <c r="R226" t="inlineStr"/>
@@ -12828,11 +11924,7 @@
       </c>
       <c r="M227" t="inlineStr"/>
       <c r="N227" t="inlineStr"/>
-      <c r="O227" t="inlineStr">
-        <is>
-          <t>08/08/2012 17:00</t>
-        </is>
-      </c>
+      <c r="O227" t="inlineStr"/>
       <c r="P227" t="inlineStr"/>
       <c r="Q227" t="inlineStr"/>
       <c r="R227" t="inlineStr"/>
@@ -12885,11 +11977,7 @@
       </c>
       <c r="M228" t="inlineStr"/>
       <c r="N228" t="inlineStr"/>
-      <c r="O228" t="inlineStr">
-        <is>
-          <t>11/10/2018 14:55</t>
-        </is>
-      </c>
+      <c r="O228" t="inlineStr"/>
       <c r="P228" t="inlineStr"/>
       <c r="Q228" t="inlineStr"/>
       <c r="R228" t="inlineStr"/>
@@ -12942,11 +12030,7 @@
       </c>
       <c r="M229" t="inlineStr"/>
       <c r="N229" t="inlineStr"/>
-      <c r="O229" t="inlineStr">
-        <is>
-          <t>10/07/2012 17:34</t>
-        </is>
-      </c>
+      <c r="O229" t="inlineStr"/>
       <c r="P229" t="inlineStr"/>
       <c r="Q229" t="inlineStr"/>
       <c r="R229" t="inlineStr"/>
@@ -12999,11 +12083,7 @@
       </c>
       <c r="M230" t="inlineStr"/>
       <c r="N230" t="inlineStr"/>
-      <c r="O230" t="inlineStr">
-        <is>
-          <t>08/12/2021 16:25</t>
-        </is>
-      </c>
+      <c r="O230" t="inlineStr"/>
       <c r="P230" t="inlineStr"/>
       <c r="Q230" t="inlineStr"/>
       <c r="R230" t="inlineStr"/>
@@ -13056,11 +12136,7 @@
       </c>
       <c r="M231" t="inlineStr"/>
       <c r="N231" t="inlineStr"/>
-      <c r="O231" t="inlineStr">
-        <is>
-          <t>11/01/2018 16:33</t>
-        </is>
-      </c>
+      <c r="O231" t="inlineStr"/>
       <c r="P231" t="inlineStr"/>
       <c r="Q231" t="inlineStr"/>
       <c r="R231" t="inlineStr"/>
@@ -13097,11 +12173,7 @@
       </c>
       <c r="M232" t="inlineStr"/>
       <c r="N232" t="inlineStr"/>
-      <c r="O232" t="inlineStr">
-        <is>
-          <t>11/07/2019 17:35</t>
-        </is>
-      </c>
+      <c r="O232" t="inlineStr"/>
       <c r="P232" t="inlineStr"/>
       <c r="Q232" t="inlineStr"/>
       <c r="R232" t="inlineStr"/>
@@ -13154,11 +12226,7 @@
       </c>
       <c r="M233" t="inlineStr"/>
       <c r="N233" t="inlineStr"/>
-      <c r="O233" t="inlineStr">
-        <is>
-          <t>13/11/2015 11:22</t>
-        </is>
-      </c>
+      <c r="O233" t="inlineStr"/>
       <c r="P233" t="inlineStr"/>
       <c r="Q233" t="inlineStr"/>
       <c r="R233" t="inlineStr"/>
@@ -13211,11 +12279,7 @@
       </c>
       <c r="M234" t="inlineStr"/>
       <c r="N234" t="inlineStr"/>
-      <c r="O234" t="inlineStr">
-        <is>
-          <t>10/06/2015 10:11</t>
-        </is>
-      </c>
+      <c r="O234" t="inlineStr"/>
       <c r="P234" t="inlineStr"/>
       <c r="Q234" t="inlineStr"/>
       <c r="R234" t="inlineStr"/>
@@ -13268,11 +12332,7 @@
       </c>
       <c r="M235" t="inlineStr"/>
       <c r="N235" t="inlineStr"/>
-      <c r="O235" t="inlineStr">
-        <is>
-          <t>17/05/2018 10:15</t>
-        </is>
-      </c>
+      <c r="O235" t="inlineStr"/>
       <c r="P235" t="inlineStr"/>
       <c r="Q235" t="inlineStr"/>
       <c r="R235" t="inlineStr"/>
@@ -13321,11 +12381,7 @@
       </c>
       <c r="M236" t="inlineStr"/>
       <c r="N236" t="inlineStr"/>
-      <c r="O236" t="inlineStr">
-        <is>
-          <t>28/08/2013 11:14</t>
-        </is>
-      </c>
+      <c r="O236" t="inlineStr"/>
       <c r="P236" t="inlineStr"/>
       <c r="Q236" t="inlineStr"/>
       <c r="R236" t="inlineStr"/>
@@ -13378,11 +12434,7 @@
       </c>
       <c r="M237" t="inlineStr"/>
       <c r="N237" t="inlineStr"/>
-      <c r="O237" t="inlineStr">
-        <is>
-          <t>16/07/2015 10:00</t>
-        </is>
-      </c>
+      <c r="O237" t="inlineStr"/>
       <c r="P237" t="inlineStr"/>
       <c r="Q237" t="inlineStr"/>
       <c r="R237" t="inlineStr"/>
@@ -13435,11 +12487,7 @@
       </c>
       <c r="M238" t="inlineStr"/>
       <c r="N238" t="inlineStr"/>
-      <c r="O238" t="inlineStr">
-        <is>
-          <t>29/11/2018 12:18</t>
-        </is>
-      </c>
+      <c r="O238" t="inlineStr"/>
       <c r="P238" t="inlineStr"/>
       <c r="Q238" t="inlineStr"/>
       <c r="R238" t="inlineStr"/>
@@ -13492,11 +12540,7 @@
       </c>
       <c r="M239" t="inlineStr"/>
       <c r="N239" t="inlineStr"/>
-      <c r="O239" t="inlineStr">
-        <is>
-          <t>22/02/2018 18:27</t>
-        </is>
-      </c>
+      <c r="O239" t="inlineStr"/>
       <c r="P239" t="inlineStr"/>
       <c r="Q239" t="inlineStr"/>
       <c r="R239" t="inlineStr"/>
@@ -13529,11 +12573,7 @@
       </c>
       <c r="M240" t="inlineStr"/>
       <c r="N240" t="inlineStr"/>
-      <c r="O240" t="inlineStr">
-        <is>
-          <t>17/04/2019 13:30</t>
-        </is>
-      </c>
+      <c r="O240" t="inlineStr"/>
       <c r="P240" t="inlineStr"/>
       <c r="Q240" t="inlineStr"/>
       <c r="R240" t="inlineStr"/>
@@ -13586,11 +12626,7 @@
       </c>
       <c r="M241" t="inlineStr"/>
       <c r="N241" t="inlineStr"/>
-      <c r="O241" t="inlineStr">
-        <is>
-          <t>21/01/2021 17:11</t>
-        </is>
-      </c>
+      <c r="O241" t="inlineStr"/>
       <c r="P241" t="inlineStr"/>
       <c r="Q241" t="inlineStr"/>
       <c r="R241" t="inlineStr"/>
@@ -13623,11 +12659,7 @@
       </c>
       <c r="M242" t="inlineStr"/>
       <c r="N242" t="inlineStr"/>
-      <c r="O242" t="inlineStr">
-        <is>
-          <t>09/08/2012 22:08</t>
-        </is>
-      </c>
+      <c r="O242" t="inlineStr"/>
       <c r="P242" t="inlineStr"/>
       <c r="Q242" t="inlineStr"/>
       <c r="R242" t="inlineStr"/>
@@ -13664,11 +12696,7 @@
       </c>
       <c r="M243" t="inlineStr"/>
       <c r="N243" t="inlineStr"/>
-      <c r="O243" t="inlineStr">
-        <is>
-          <t>06/01/2017 09:44</t>
-        </is>
-      </c>
+      <c r="O243" t="inlineStr"/>
       <c r="P243" t="inlineStr"/>
       <c r="Q243" t="inlineStr"/>
       <c r="R243" t="inlineStr"/>
@@ -13701,11 +12729,7 @@
       </c>
       <c r="M244" t="inlineStr"/>
       <c r="N244" t="inlineStr"/>
-      <c r="O244" t="inlineStr">
-        <is>
-          <t>27/12/2013 08:55</t>
-        </is>
-      </c>
+      <c r="O244" t="inlineStr"/>
       <c r="P244" t="inlineStr"/>
       <c r="Q244" t="inlineStr"/>
       <c r="R244" t="inlineStr"/>
@@ -13758,11 +12782,7 @@
       </c>
       <c r="M245" t="inlineStr"/>
       <c r="N245" t="inlineStr"/>
-      <c r="O245" t="inlineStr">
-        <is>
-          <t>06/05/2021 17:45</t>
-        </is>
-      </c>
+      <c r="O245" t="inlineStr"/>
       <c r="P245" t="inlineStr"/>
       <c r="Q245" t="inlineStr"/>
       <c r="R245" t="inlineStr"/>
@@ -13795,11 +12815,7 @@
       </c>
       <c r="M246" t="inlineStr"/>
       <c r="N246" t="inlineStr"/>
-      <c r="O246" t="inlineStr">
-        <is>
-          <t>29/01/2014 11:50</t>
-        </is>
-      </c>
+      <c r="O246" t="inlineStr"/>
       <c r="P246" t="inlineStr"/>
       <c r="Q246" t="inlineStr"/>
       <c r="R246" t="inlineStr"/>
@@ -13832,11 +12848,7 @@
       </c>
       <c r="M247" t="inlineStr"/>
       <c r="N247" t="inlineStr"/>
-      <c r="O247" t="inlineStr">
-        <is>
-          <t>30/09/2014 15:40</t>
-        </is>
-      </c>
+      <c r="O247" t="inlineStr"/>
       <c r="P247" t="inlineStr"/>
       <c r="Q247" t="inlineStr"/>
       <c r="R247" t="inlineStr"/>
@@ -13869,11 +12881,7 @@
       </c>
       <c r="M248" t="inlineStr"/>
       <c r="N248" t="inlineStr"/>
-      <c r="O248" t="inlineStr">
-        <is>
-          <t>30/12/2013 14:44</t>
-        </is>
-      </c>
+      <c r="O248" t="inlineStr"/>
       <c r="P248" t="inlineStr"/>
       <c r="Q248" t="inlineStr"/>
       <c r="R248" t="inlineStr"/>
@@ -13906,11 +12914,7 @@
       </c>
       <c r="M249" t="inlineStr"/>
       <c r="N249" t="inlineStr"/>
-      <c r="O249" t="inlineStr">
-        <is>
-          <t>18/09/2013 10:27</t>
-        </is>
-      </c>
+      <c r="O249" t="inlineStr"/>
       <c r="P249" t="inlineStr"/>
       <c r="Q249" t="inlineStr"/>
       <c r="R249" t="inlineStr"/>
@@ -13943,11 +12947,7 @@
       </c>
       <c r="M250" t="inlineStr"/>
       <c r="N250" t="inlineStr"/>
-      <c r="O250" t="inlineStr">
-        <is>
-          <t>27/09/2013 16:39</t>
-        </is>
-      </c>
+      <c r="O250" t="inlineStr"/>
       <c r="P250" t="inlineStr"/>
       <c r="Q250" t="inlineStr"/>
       <c r="R250" t="inlineStr"/>
@@ -13980,11 +12980,7 @@
       </c>
       <c r="M251" t="inlineStr"/>
       <c r="N251" t="inlineStr"/>
-      <c r="O251" t="inlineStr">
-        <is>
-          <t>27/12/2013 09:45</t>
-        </is>
-      </c>
+      <c r="O251" t="inlineStr"/>
       <c r="P251" t="inlineStr"/>
       <c r="Q251" t="inlineStr"/>
       <c r="R251" t="inlineStr"/>
@@ -14017,11 +13013,7 @@
       </c>
       <c r="M252" t="inlineStr"/>
       <c r="N252" t="inlineStr"/>
-      <c r="O252" t="inlineStr">
-        <is>
-          <t>19/09/2013 14:14</t>
-        </is>
-      </c>
+      <c r="O252" t="inlineStr"/>
       <c r="P252" t="inlineStr"/>
       <c r="Q252" t="inlineStr"/>
       <c r="R252" t="inlineStr"/>
@@ -14054,11 +13046,7 @@
       </c>
       <c r="M253" t="inlineStr"/>
       <c r="N253" t="inlineStr"/>
-      <c r="O253" t="inlineStr">
-        <is>
-          <t>17/02/2014 08:34</t>
-        </is>
-      </c>
+      <c r="O253" t="inlineStr"/>
       <c r="P253" t="inlineStr"/>
       <c r="Q253" t="inlineStr"/>
       <c r="R253" t="inlineStr"/>
@@ -14091,11 +13079,7 @@
       </c>
       <c r="M254" t="inlineStr"/>
       <c r="N254" t="inlineStr"/>
-      <c r="O254" t="inlineStr">
-        <is>
-          <t>03/09/2014 10:32</t>
-        </is>
-      </c>
+      <c r="O254" t="inlineStr"/>
       <c r="P254" t="inlineStr"/>
       <c r="Q254" t="inlineStr"/>
       <c r="R254" t="inlineStr"/>
@@ -14128,11 +13112,7 @@
       </c>
       <c r="M255" t="inlineStr"/>
       <c r="N255" t="inlineStr"/>
-      <c r="O255" t="inlineStr">
-        <is>
-          <t>28/01/2014 13:20</t>
-        </is>
-      </c>
+      <c r="O255" t="inlineStr"/>
       <c r="P255" t="inlineStr"/>
       <c r="Q255" t="inlineStr"/>
       <c r="R255" t="inlineStr"/>

</xml_diff>